<commit_message>
Analiza Izob_na_domu, delno OŠ. Rahlo popravljeni podatki. Narejena mapa.
</commit_message>
<xml_diff>
--- a/podatki/Izob_na_domu.xlsx
+++ b/podatki/Izob_na_domu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="Izob_na_domu.csv" sheetId="1" r:id="rId1"/>
@@ -389,8 +389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F874" sqref="F874"/>
+    <sheetView tabSelected="1" topLeftCell="A1073" workbookViewId="0">
+      <selection activeCell="H876" sqref="H876"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17886,7 +17886,7 @@
         <v>17</v>
       </c>
       <c r="D875" s="1">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="E875" s="1" t="s">
         <v>14</v>

</xml_diff>